<commit_message>
updated schedule - Ragab
</commit_message>
<xml_diff>
--- a/Project schedule (PS_DOC_2).xlsx
+++ b/Project schedule (PS_DOC_2).xlsx
@@ -134,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -155,13 +155,23 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -176,15 +186,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -202,11 +212,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,8 +535,33 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16">
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
     </row>
     <row r="17">
       <c r="E17" s="7"/>

</xml_diff>